<commit_message>
skew binomial passing cpp test
</commit_message>
<xml_diff>
--- a/xls/american.xlsx
+++ b/xls/american.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\FRE6233\Spring2023\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1BA85C-66C7-4284-8FB5-400EB8E021E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EBE217-0715-430B-B61F-DEFAB00772AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>f</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>europeanp</t>
   </si>
 </sst>
 </file>
@@ -1862,7 +1865,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1938,14 +1943,17 @@
         <v>80</v>
       </c>
       <c r="G7" s="4" cm="1">
-        <f t="array" ref="G7:G47">_xlfn.MAP(_xlfn.ANCHORARRAY(F7), _xlfn.LAMBDA(_xlpm.k, _xll.XLL.BINOMIAL.EUROPEAN(f, s, -_xlpm.k, n)))</f>
+        <f t="array" ref="G7:G47">_xlfn.MAP(_xlfn.ANCHORARRAY(F7), _xlfn.LAMBDA(_xlpm.ki, _xll.XLL.BINOMIAL.EUROPEAN(f, s, -_xlpm.ki, n)))</f>
         <v>3.9875882204585225E-2</v>
       </c>
       <c r="H7" s="4" cm="1">
-        <f t="array" ref="H7:H47">_xlfn.MAP(_xlfn.ANCHORARRAY(G7),_xlfn.ANCHORARRAY( F7), _xlfn.LAMBDA(_xlpm.p,_xlpm.k, _xll.BLACK.PUT.IMPLIED(f, _xlpm.p, _xlpm.k)))</f>
+        <f t="array" ref="H7:H47">_xlfn.MAP(_xlfn.ANCHORARRAY(G7),_xlfn.ANCHORARRAY( F7), _xlfn.LAMBDA(_xlpm.pi,_xlpm.ki, _xll.BLACK.PUT.IMPLIED(f, _xlpm.pi, ABS(_xlpm.ki))))</f>
         <v>9.9986983515938099E-2</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="4" cm="1">
+        <f t="array" ref="I7:I47">_xlfn.MAP(_xlfn.ANCHORARRAY(F7), _xlfn.LAMBDA(_xlpm.k, _xll.XLL.BINOMIAL.EUROPEANP(f, s, -_xlpm.k, n, p)))</f>
+        <v>0</v>
+      </c>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -1965,10 +1973,19 @@
       <c r="H8" s="4">
         <v>9.9991303766673548E-2</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" cm="1">
+        <f t="array" ref="C9">_xll.XLL.BINOMIAL.EUROPEANP(f, s, k, n, p)</f>
+        <v>1.2581009387082853E-2</v>
+      </c>
       <c r="F9">
         <v>82</v>
       </c>
@@ -1978,7 +1995,9 @@
       <c r="H9" s="4">
         <v>9.9994151277397109E-2</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -1991,7 +2010,9 @@
       <c r="H10" s="4">
         <v>9.9993777166791004E-2</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7">
+        <v>0</v>
+      </c>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -2004,7 +2025,9 @@
       <c r="H11" s="4">
         <v>9.9987765853972482E-2</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -2017,7 +2040,9 @@
       <c r="H12" s="4">
         <v>9.9973056427929918E-2</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7">
+        <v>0</v>
+      </c>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -2030,7 +2055,9 @@
       <c r="H13" s="4">
         <v>9.9968777298421144E-2</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -2043,7 +2070,9 @@
       <c r="H14" s="4">
         <v>9.9995729779350104E-2</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="I14" s="7">
+        <v>0</v>
+      </c>
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -2056,7 +2085,9 @@
       <c r="H15" s="4">
         <v>0.10001193360435243</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -2069,7 +2100,9 @@
       <c r="H16" s="4">
         <v>0.10001214105216549</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="7">
+        <v>0</v>
+      </c>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="6:10" x14ac:dyDescent="0.25">
@@ -2082,7 +2115,9 @@
       <c r="H17" s="4">
         <v>9.999059045391448E-2</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="7">
+        <v>0</v>
+      </c>
       <c r="J17" s="7"/>
     </row>
     <row r="18" spans="6:10" x14ac:dyDescent="0.25">
@@ -2095,7 +2130,9 @@
       <c r="H18" s="4">
         <v>9.9990003863038759E-2</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="7">
+        <v>0</v>
+      </c>
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="6:10" x14ac:dyDescent="0.25">
@@ -2108,7 +2145,9 @@
       <c r="H19" s="4">
         <v>0.10001799335501931</v>
       </c>
-      <c r="I19" s="7"/>
+      <c r="I19" s="7">
+        <v>0</v>
+      </c>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="6:10" x14ac:dyDescent="0.25">
@@ -2121,7 +2160,9 @@
       <c r="H20" s="4">
         <v>0.10001515909179724</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="7">
+        <v>0</v>
+      </c>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="6:10" x14ac:dyDescent="0.25">
@@ -2134,7 +2175,9 @@
       <c r="H21" s="4">
         <v>9.9974144216051802E-2</v>
       </c>
-      <c r="I21" s="7"/>
+      <c r="I21" s="7">
+        <v>0</v>
+      </c>
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="6:10" x14ac:dyDescent="0.25">
@@ -2147,7 +2190,9 @@
       <c r="H22" s="4">
         <v>0.10001684118825498</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="7">
+        <v>0</v>
+      </c>
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="6:10" x14ac:dyDescent="0.25">
@@ -2160,7 +2205,9 @@
       <c r="H23" s="4">
         <v>0.10001889748366183</v>
       </c>
-      <c r="I23" s="7"/>
+      <c r="I23" s="7">
+        <v>0</v>
+      </c>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="6:10" x14ac:dyDescent="0.25">
@@ -2173,7 +2220,9 @@
       <c r="H24" s="4">
         <v>9.9979521651878525E-2</v>
       </c>
-      <c r="I24" s="7"/>
+      <c r="I24" s="7">
+        <v>0</v>
+      </c>
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="6:10" x14ac:dyDescent="0.25">
@@ -2186,7 +2235,9 @@
       <c r="H25" s="4">
         <v>0.10002296148539916</v>
       </c>
-      <c r="I25" s="7"/>
+      <c r="I25" s="7">
+        <v>0</v>
+      </c>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="6:10" x14ac:dyDescent="0.25">
@@ -2199,7 +2250,9 @@
       <c r="H26" s="4">
         <v>0.10000715449212727</v>
       </c>
-      <c r="I26" s="7"/>
+      <c r="I26" s="7">
+        <v>0</v>
+      </c>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="6:10" x14ac:dyDescent="0.25">
@@ -2212,7 +2265,9 @@
       <c r="H27" s="4">
         <v>0.10000796850078694</v>
       </c>
-      <c r="I27" s="7"/>
+      <c r="I27" s="7">
+        <v>1.2581009387082853E-2</v>
+      </c>
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="6:10" x14ac:dyDescent="0.25">
@@ -2225,7 +2280,9 @@
       <c r="H28" s="4">
         <v>0.10002087460031353</v>
       </c>
-      <c r="I28" s="7"/>
+      <c r="I28" s="7">
+        <v>6.5453444748816064E-2</v>
+      </c>
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="6:10" x14ac:dyDescent="0.25">
@@ -2238,7 +2295,9 @@
       <c r="H29" s="4">
         <v>9.9988692618370748E-2</v>
       </c>
-      <c r="I29" s="7"/>
+      <c r="I29" s="7">
+        <v>0.15556484329170647</v>
+      </c>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="6:10" x14ac:dyDescent="0.25">
@@ -2251,7 +2310,9 @@
       <c r="H30" s="4">
         <v>0.10002335873483793</v>
       </c>
-      <c r="I30" s="7"/>
+      <c r="I30" s="7">
+        <v>0.28620621826235682</v>
+      </c>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="6:10" x14ac:dyDescent="0.25">
@@ -2264,7 +2325,9 @@
       <c r="H31" s="4">
         <v>9.9974537610444891E-2</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="7">
+        <v>0.45010034988836661</v>
+      </c>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="6:10" x14ac:dyDescent="0.25">
@@ -2277,7 +2340,9 @@
       <c r="H32" s="4">
         <v>0.10002206120026627</v>
       </c>
-      <c r="I32" s="7"/>
+      <c r="I32" s="7">
+        <v>0.65238369501277815</v>
+      </c>
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.25">
@@ -2290,7 +2355,9 @@
       <c r="H33" s="4">
         <v>9.997177833919875E-2</v>
       </c>
-      <c r="I33" s="7"/>
+      <c r="I33" s="7">
+        <v>0.88399659013774623</v>
+      </c>
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="6:10" x14ac:dyDescent="0.25">
@@ -2303,7 +2370,9 @@
       <c r="H34" s="4">
         <v>0.10001987180142768</v>
       </c>
-      <c r="I34" s="7"/>
+      <c r="I34" s="7">
+        <v>1.149814808385905</v>
+      </c>
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="6:10" x14ac:dyDescent="0.25">
@@ -2316,7 +2385,9 @@
       <c r="H35" s="4">
         <v>9.9976579689776746E-2</v>
       </c>
-      <c r="I35" s="7"/>
+      <c r="I35" s="7">
+        <v>1.4412614890950577</v>
+      </c>
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="6:10" x14ac:dyDescent="0.25">
@@ -2329,7 +2400,9 @@
       <c r="H36" s="4">
         <v>0.10001568903124339</v>
       </c>
-      <c r="I36" s="7"/>
+      <c r="I36" s="7">
+        <v>1.7616516934244075</v>
+      </c>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="6:10" x14ac:dyDescent="0.25">
@@ -2342,7 +2415,9 @@
       <c r="H37" s="4">
         <v>9.9990059899305428E-2</v>
       </c>
-      <c r="I37" s="7"/>
+      <c r="I37" s="7">
+        <v>2.1043110834848981</v>
+      </c>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="6:10" x14ac:dyDescent="0.25">
@@ -2355,7 +2430,9 @@
       <c r="H38" s="4">
         <v>0.10000495344650021</v>
       </c>
-      <c r="I38" s="7"/>
+      <c r="I38" s="7">
+        <v>2.4700028473319504</v>
+      </c>
       <c r="J38" s="7"/>
     </row>
     <row r="39" spans="6:10" x14ac:dyDescent="0.25">
@@ -2368,7 +2445,9 @@
       <c r="H39" s="4">
         <v>0.10000390601572311</v>
       </c>
-      <c r="I39" s="7"/>
+      <c r="I39" s="7">
+        <v>2.8550481011426192</v>
+      </c>
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="6:10" x14ac:dyDescent="0.25">
@@ -2381,7 +2460,9 @@
       <c r="H40" s="4">
         <v>9.9980294762008787E-2</v>
       </c>
-      <c r="I40" s="7"/>
+      <c r="I40" s="7">
+        <v>3.2573411312079492</v>
+      </c>
       <c r="J40" s="7"/>
     </row>
     <row r="41" spans="6:10" x14ac:dyDescent="0.25">
@@ -2394,7 +2475,9 @@
       <c r="H41" s="4">
         <v>0.10000837172783798</v>
       </c>
-      <c r="I41" s="7"/>
+      <c r="I41" s="7">
+        <v>3.6763909500119594</v>
+      </c>
       <c r="J41" s="7"/>
     </row>
     <row r="42" spans="6:10" x14ac:dyDescent="0.25">
@@ -2407,7 +2490,9 @@
       <c r="H42" s="4">
         <v>9.9976444811474455E-2</v>
       </c>
-      <c r="I42" s="7"/>
+      <c r="I42" s="7">
+        <v>4.108249901850737</v>
+      </c>
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="6:10" x14ac:dyDescent="0.25">
@@ -2420,7 +2505,9 @@
       <c r="H43" s="4">
         <v>9.9991709294954767E-2</v>
       </c>
-      <c r="I43" s="7"/>
+      <c r="I43" s="7">
+        <v>4.553077545690118</v>
+      </c>
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="6:10" x14ac:dyDescent="0.25">
@@ -2433,7 +2520,9 @@
       <c r="H44" s="4">
         <v>9.9999402560396661E-2</v>
       </c>
-      <c r="I44" s="7"/>
+      <c r="I44" s="7">
+        <v>5.0083680726050144</v>
+      </c>
       <c r="J44" s="7"/>
     </row>
     <row r="45" spans="6:10" x14ac:dyDescent="0.25">
@@ -2446,7 +2535,9 @@
       <c r="H45" s="4">
         <v>9.9957024662366764E-2</v>
       </c>
-      <c r="I45" s="7"/>
+      <c r="I45" s="7">
+        <v>5.4722742152426456</v>
+      </c>
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="6:10" x14ac:dyDescent="0.25">
@@ -2459,7 +2550,9 @@
       <c r="H46" s="4">
         <v>9.9987694861247076E-2</v>
       </c>
-      <c r="I46" s="7"/>
+      <c r="I46" s="7">
+        <v>5.9449123446700609</v>
+      </c>
       <c r="J46" s="7"/>
     </row>
     <row r="47" spans="6:10" x14ac:dyDescent="0.25">
@@ -2472,7 +2565,9 @@
       <c r="H47" s="4">
         <v>9.9991734781377892E-2</v>
       </c>
-      <c r="I47" s="7"/>
+      <c r="I47" s="7">
+        <v>6.4240163435446345</v>
+      </c>
       <c r="J47" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
skew binomial for xll working?
</commit_message>
<xml_diff>
--- a/xls/american.xlsx
+++ b/xls/american.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\FRE6233\Spring2023\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EBE217-0715-430B-B61F-DEFAB00772AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FD580D-1BC8-4E98-8F6D-3B6609E34E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -739,6 +739,129 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
+                <c:pt idx="0" formatCode="0.00000">
+                  <c:v>8.004546881985547E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9280025055275705E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8464919706949909E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7593990166917426E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6659894338769283E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5654003394973954E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4579940422953531E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.3455912786980951E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2233836567506829E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0898389854515784E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.943168560326278E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.7847159795867973E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6139966863034999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.4235355219753792E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.2096825138379781E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9776142309016539E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.7132316094029564E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4083682098214986E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.0627727094427012E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.6481595276886251E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.1400924754334996E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.473865365935782E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4070771828348839E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1866,7 +1989,7 @@
   <dimension ref="B2:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,7 +2021,7 @@
         <v>10</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -1951,10 +2074,13 @@
         <v>9.9986983515938099E-2</v>
       </c>
       <c r="I7" s="4" cm="1">
-        <f t="array" ref="I7:I47">_xlfn.MAP(_xlfn.ANCHORARRAY(F7), _xlfn.LAMBDA(_xlpm.k, _xll.XLL.BINOMIAL.EUROPEANP(f, s, -_xlpm.k, n, p)))</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="7"/>
+        <f t="array" ref="I7:I47">_xlfn.MAP(_xlfn.ANCHORARRAY(F7), _xlfn.LAMBDA(_xlpm.ki, _xll.XLL.BINOMIAL.EUROPEANP(f, s, -_xlpm.ki, n, p)))</f>
+        <v>5.6742680794259516E-3</v>
+      </c>
+      <c r="J7" s="4" cm="1">
+        <f t="array" ref="J7:J47">_xlfn.MAP(_xlfn.ANCHORARRAY(I7),_xlfn.ANCHORARRAY( F7), _xlfn.LAMBDA(_xlpm.pi,_xlpm.ki, _xll.BLACK.PUT.IMPLIED(f, _xlpm.pi, ABS(_xlpm.ki))))</f>
+        <v>8.004546881985547E-2</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -1974,9 +2100,11 @@
         <v>9.9991303766673548E-2</v>
       </c>
       <c r="I8" s="7">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7"/>
+        <v>8.6672857699351541E-3</v>
+      </c>
+      <c r="J8" s="7">
+        <v>7.9280025055275705E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -1984,7 +2112,7 @@
       </c>
       <c r="C9" s="2" cm="1">
         <f t="array" ref="C9">_xll.XLL.BINOMIAL.EUROPEANP(f, s, k, n, p)</f>
-        <v>1.2581009387082853E-2</v>
+        <v>1.6515399823829906</v>
       </c>
       <c r="F9">
         <v>82</v>
@@ -1996,9 +2124,11 @@
         <v>9.9994151277397109E-2</v>
       </c>
       <c r="I9" s="7">
-        <v>0</v>
-      </c>
-      <c r="J9" s="7"/>
+        <v>1.2996437340330881E-2</v>
+      </c>
+      <c r="J9" s="7">
+        <v>7.8464919706949909E-2</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F10">
@@ -2011,9 +2141,11 @@
         <v>9.9993777166791004E-2</v>
       </c>
       <c r="I10" s="7">
-        <v>0</v>
-      </c>
-      <c r="J10" s="7"/>
+        <v>1.9141819021865361E-2</v>
+      </c>
+      <c r="J10" s="7">
+        <v>7.7593990166917426E-2</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F11">
@@ -2026,9 +2158,11 @@
         <v>9.9987765853972482E-2</v>
       </c>
       <c r="I11" s="7">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7"/>
+        <v>2.770710419940239E-2</v>
+      </c>
+      <c r="J11" s="7">
+        <v>7.6659894338769283E-2</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F12">
@@ -2041,9 +2175,11 @@
         <v>9.9973056427929918E-2</v>
       </c>
       <c r="I12" s="7">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7"/>
+        <v>3.9433720244447509E-2</v>
+      </c>
+      <c r="J12" s="7">
+        <v>7.5654003394973954E-2</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F13">
@@ -2056,9 +2192,11 @@
         <v>9.9968777298421144E-2</v>
       </c>
       <c r="I13" s="7">
-        <v>0</v>
-      </c>
-      <c r="J13" s="7"/>
+        <v>5.527649766283145E-2</v>
+      </c>
+      <c r="J13" s="7">
+        <v>7.4579940422953531E-2</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F14">
@@ -2071,9 +2209,11 @@
         <v>9.9995729779350104E-2</v>
       </c>
       <c r="I14" s="7">
-        <v>0</v>
-      </c>
-      <c r="J14" s="7"/>
+        <v>7.6517593906369558E-2</v>
+      </c>
+      <c r="J14" s="7">
+        <v>7.3455912786980951E-2</v>
+      </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F15">
@@ -2086,9 +2226,11 @@
         <v>0.10001193360435243</v>
       </c>
       <c r="I15" s="7">
-        <v>0</v>
-      </c>
-      <c r="J15" s="7"/>
+        <v>0.10430462026511235</v>
+      </c>
+      <c r="J15" s="7">
+        <v>7.2233836567506829E-2</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F16">
@@ -2101,9 +2243,11 @@
         <v>0.10001214105216549</v>
       </c>
       <c r="I16" s="7">
-        <v>0</v>
-      </c>
-      <c r="J16" s="7"/>
+        <v>0.14007305256249702</v>
+      </c>
+      <c r="J16" s="7">
+        <v>7.0898389854515784E-2</v>
+      </c>
     </row>
     <row r="17" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F17">
@@ -2116,9 +2260,11 @@
         <v>9.999059045391448E-2</v>
       </c>
       <c r="I17" s="7">
-        <v>0</v>
-      </c>
-      <c r="J17" s="7"/>
+        <v>0.18540016987196328</v>
+      </c>
+      <c r="J17" s="7">
+        <v>6.943168560326278E-2</v>
+      </c>
     </row>
     <row r="18" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F18">
@@ -2131,9 +2277,11 @@
         <v>9.9990003863038759E-2</v>
       </c>
       <c r="I18" s="7">
-        <v>0</v>
-      </c>
-      <c r="J18" s="7"/>
+        <v>0.24247612312389463</v>
+      </c>
+      <c r="J18" s="7">
+        <v>6.7847159795867973E-2</v>
+      </c>
     </row>
     <row r="19" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F19">
@@ -2146,9 +2294,11 @@
         <v>0.10001799335501931</v>
       </c>
       <c r="I19" s="7">
-        <v>0</v>
-      </c>
-      <c r="J19" s="7"/>
+        <v>0.31370668379329214</v>
+      </c>
+      <c r="J19" s="7">
+        <v>6.6139966863034999E-2</v>
+      </c>
     </row>
     <row r="20" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F20">
@@ -2161,9 +2311,11 @@
         <v>0.10001515909179724</v>
       </c>
       <c r="I20" s="7">
-        <v>0</v>
-      </c>
-      <c r="J20" s="7"/>
+        <v>0.4005149799128917</v>
+      </c>
+      <c r="J20" s="7">
+        <v>6.4235355219753792E-2</v>
+      </c>
     </row>
     <row r="21" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F21">
@@ -2176,9 +2328,11 @@
         <v>9.9974144216051802E-2</v>
       </c>
       <c r="I21" s="7">
-        <v>0</v>
-      </c>
-      <c r="J21" s="7"/>
+        <v>0.50486258740540424</v>
+      </c>
+      <c r="J21" s="7">
+        <v>6.2096825138379781E-2</v>
+      </c>
     </row>
     <row r="22" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F22">
@@ -2191,9 +2345,11 @@
         <v>0.10001684118825498</v>
       </c>
       <c r="I22" s="7">
-        <v>0</v>
-      </c>
-      <c r="J22" s="7"/>
+        <v>0.63128984517234121</v>
+      </c>
+      <c r="J22" s="7">
+        <v>5.9776142309016539E-2</v>
+      </c>
     </row>
     <row r="23" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F23">
@@ -2206,9 +2362,11 @@
         <v>0.10001889748366183</v>
       </c>
       <c r="I23" s="7">
-        <v>0</v>
-      </c>
-      <c r="J23" s="7"/>
+        <v>0.78015039562040145</v>
+      </c>
+      <c r="J23" s="7">
+        <v>5.7132316094029564E-2</v>
+      </c>
     </row>
     <row r="24" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F24">
@@ -2221,9 +2379,11 @@
         <v>9.9979521651878525E-2</v>
       </c>
       <c r="I24" s="7">
-        <v>0</v>
-      </c>
-      <c r="J24" s="7"/>
+        <v>0.95326230555520719</v>
+      </c>
+      <c r="J24" s="7">
+        <v>5.4083682098214986E-2</v>
+      </c>
     </row>
     <row r="25" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F25">
@@ -2236,9 +2396,11 @@
         <v>0.10002296148539916</v>
       </c>
       <c r="I25" s="7">
-        <v>0</v>
-      </c>
-      <c r="J25" s="7"/>
+        <v>1.1564077050154515</v>
+      </c>
+      <c r="J25" s="7">
+        <v>5.0627727094427012E-2</v>
+      </c>
     </row>
     <row r="26" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F26">
@@ -2251,9 +2413,11 @@
         <v>0.10000715449212727</v>
       </c>
       <c r="I26" s="7">
-        <v>0</v>
-      </c>
-      <c r="J26" s="7"/>
+        <v>1.387860612919777</v>
+      </c>
+      <c r="J26" s="7">
+        <v>4.6481595276886251E-2</v>
+      </c>
     </row>
     <row r="27" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F27">
@@ -2266,9 +2430,11 @@
         <v>0.10000796850078694</v>
       </c>
       <c r="I27" s="7">
-        <v>1.2581009387082853E-2</v>
-      </c>
-      <c r="J27" s="7"/>
+        <v>1.6515399823829906</v>
+      </c>
+      <c r="J27" s="7">
+        <v>4.1400924754334996E-2</v>
+      </c>
     </row>
     <row r="28" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F28">
@@ -2281,9 +2447,11 @@
         <v>0.10002087460031353</v>
       </c>
       <c r="I28" s="7">
-        <v>6.5453444748816064E-2</v>
-      </c>
-      <c r="J28" s="7"/>
+        <v>1.9494702817872109</v>
+      </c>
+      <c r="J28" s="7">
+        <v>3.473865365935782E-2</v>
+      </c>
     </row>
     <row r="29" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F29">
@@ -2296,9 +2464,11 @@
         <v>9.9988692618370748E-2</v>
       </c>
       <c r="I29" s="7">
-        <v>0.15556484329170647</v>
-      </c>
-      <c r="J29" s="7"/>
+        <v>2.2807126102039654</v>
+      </c>
+      <c r="J29" s="7">
+        <v>2.4070771828348839E-2</v>
+      </c>
     </row>
     <row r="30" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F30">
@@ -2311,9 +2481,11 @@
         <v>0.10002335873483793</v>
       </c>
       <c r="I30" s="7">
-        <v>0.28620621826235682</v>
-      </c>
-      <c r="J30" s="7"/>
+        <v>2.6509403085409886</v>
+      </c>
+      <c r="J30" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="31" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F31">
@@ -2326,9 +2498,11 @@
         <v>9.9974537610444891E-2</v>
       </c>
       <c r="I31" s="7">
-        <v>0.45010034988836661</v>
-      </c>
-      <c r="J31" s="7"/>
+        <v>3.0548641311781184</v>
+      </c>
+      <c r="J31" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="32" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F32">
@@ -2341,9 +2515,11 @@
         <v>0.10002206120026627</v>
       </c>
       <c r="I32" s="7">
-        <v>0.65238369501277815</v>
-      </c>
-      <c r="J32" s="7"/>
+        <v>3.5004770844639719</v>
+      </c>
+      <c r="J32" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F33">
@@ -2356,9 +2532,11 @@
         <v>9.997177833919875E-2</v>
       </c>
       <c r="I33" s="7">
-        <v>0.88399659013774623</v>
-      </c>
-      <c r="J33" s="7"/>
+        <v>3.9798220573982244</v>
+      </c>
+      <c r="J33" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="34" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F34">
@@ -2371,9 +2549,11 @@
         <v>0.10001987180142768</v>
       </c>
       <c r="I34" s="7">
-        <v>1.149814808385905</v>
-      </c>
-      <c r="J34" s="7"/>
+        <v>4.5007937109665539</v>
+      </c>
+      <c r="J34" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="35" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F35">
@@ -2386,9 +2566,11 @@
         <v>9.9976579689776746E-2</v>
       </c>
       <c r="I35" s="7">
-        <v>1.4412614890950577</v>
-      </c>
-      <c r="J35" s="7"/>
+        <v>5.0549839574415554</v>
+      </c>
+      <c r="J35" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="36" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F36">
@@ -2401,9 +2583,11 @@
         <v>0.10001568903124339</v>
       </c>
       <c r="I36" s="7">
-        <v>1.7616516934244075</v>
-      </c>
-      <c r="J36" s="7"/>
+        <v>5.6490713580716427</v>
+      </c>
+      <c r="J36" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="37" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F37">
@@ -2416,9 +2600,11 @@
         <v>9.9990059899305428E-2</v>
       </c>
       <c r="I37" s="7">
-        <v>2.1043110834848981</v>
-      </c>
-      <c r="J37" s="7"/>
+        <v>6.2754832404295566</v>
+      </c>
+      <c r="J37" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="38" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F38">
@@ -2431,9 +2617,11 @@
         <v>0.10000495344650021</v>
       </c>
       <c r="I38" s="7">
-        <v>2.4700028473319504</v>
-      </c>
-      <c r="J38" s="7"/>
+        <v>6.9375479959285729</v>
+      </c>
+      <c r="J38" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="39" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F39">
@@ -2446,9 +2634,11 @@
         <v>0.10000390601572311</v>
       </c>
       <c r="I39" s="7">
-        <v>2.8550481011426192</v>
-      </c>
-      <c r="J39" s="7"/>
+        <v>7.6311182814945369</v>
+      </c>
+      <c r="J39" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="40" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F40">
@@ -2461,9 +2651,11 @@
         <v>9.9980294762008787E-2</v>
       </c>
       <c r="I40" s="7">
-        <v>3.2573411312079492</v>
-      </c>
-      <c r="J40" s="7"/>
+        <v>8.354582494797004</v>
+      </c>
+      <c r="J40" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="41" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F41">
@@ -2476,9 +2668,11 @@
         <v>0.10000837172783798</v>
       </c>
       <c r="I41" s="7">
-        <v>3.6763909500119594</v>
-      </c>
-      <c r="J41" s="7"/>
+        <v>9.1085853668896313</v>
+      </c>
+      <c r="J41" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="42" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F42">
@@ -2491,9 +2685,11 @@
         <v>9.9976444811474455E-2</v>
       </c>
       <c r="I42" s="7">
-        <v>4.108249901850737</v>
-      </c>
-      <c r="J42" s="7"/>
+        <v>9.8873548311942585</v>
+      </c>
+      <c r="J42" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="43" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F43">
@@ -2506,9 +2702,11 @@
         <v>9.9991709294954767E-2</v>
       </c>
       <c r="I43" s="7">
-        <v>4.553077545690118</v>
-      </c>
-      <c r="J43" s="7"/>
+        <v>10.692680441340039</v>
+      </c>
+      <c r="J43" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="44" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F44">
@@ -2521,9 +2719,11 @@
         <v>9.9999402560396661E-2</v>
       </c>
       <c r="I44" s="7">
-        <v>5.0083680726050144</v>
-      </c>
-      <c r="J44" s="7"/>
+        <v>11.520531923807338</v>
+      </c>
+      <c r="J44" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="45" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F45">
@@ -2536,9 +2736,11 @@
         <v>9.9957024662366764E-2</v>
       </c>
       <c r="I45" s="7">
-        <v>5.4722742152426456</v>
-      </c>
-      <c r="J45" s="7"/>
+        <v>12.367978276005202</v>
+      </c>
+      <c r="J45" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="46" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F46">
@@ -2551,9 +2753,11 @@
         <v>9.9987694861247076E-2</v>
       </c>
       <c r="I46" s="7">
-        <v>5.9449123446700609</v>
-      </c>
-      <c r="J46" s="7"/>
+        <v>13.236455620729942</v>
+      </c>
+      <c r="J46" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="47" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F47">
@@ -2566,9 +2770,11 @@
         <v>9.9991734781377892E-2</v>
       </c>
       <c r="I47" s="7">
-        <v>6.4240163435446345</v>
-      </c>
-      <c r="J47" s="7"/>
+        <v>14.121314738754389</v>
+      </c>
+      <c r="J47" s="7" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>